<commit_message>
Updation related to bookcreation and credentials.java
</commit_message>
<xml_diff>
--- a/KitabooAutomation/testData/platformConfig.xlsx
+++ b/KitabooAutomation/testData/platformConfig.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="userConfig" sheetId="2" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="3" r:id="rId2"/>
+    <sheet name="CreateBook" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t>Environment</t>
   </si>
@@ -26,7 +27,7 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>All Browsers</t>
+    <t>Chrome</t>
   </si>
   <si>
     <t>Module</t>
@@ -59,12 +60,15 @@
     <t>US</t>
   </si>
   <si>
-    <t>Staging</t>
+    <t>Distribution</t>
   </si>
   <si>
     <t>EPUB</t>
   </si>
   <si>
+    <t>Stag</t>
+  </si>
+  <si>
     <t>https://qacreate.kitaboo.com/home.xhtml</t>
   </si>
   <si>
@@ -77,13 +81,10 @@
     <t>automation.kitaboo@yopmail.com</t>
   </si>
   <si>
-    <t>Distribution</t>
-  </si>
-  <si>
     <t>automation.dis@yopmail.com</t>
   </si>
   <si>
-    <t>Production</t>
+    <t>ProdUS</t>
   </si>
   <si>
     <t>https://create.kitaboo.com/home.xhtml</t>
@@ -98,6 +99,9 @@
     <t>automation.test1@yopmail.com</t>
   </si>
   <si>
+    <t>ProdEU</t>
+  </si>
+  <si>
     <t>https://create.kitaboo.eu/home.xhtml</t>
   </si>
   <si>
@@ -117,6 +121,102 @@
   </si>
   <si>
     <t>Execution</t>
+  </si>
+  <si>
+    <t>Ttile</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Book Type</t>
+  </si>
+  <si>
+    <t>Book Oriantaion</t>
+  </si>
+  <si>
+    <t>Font Permission</t>
+  </si>
+  <si>
+    <t>DPI</t>
+  </si>
+  <si>
+    <t>Show Folio</t>
+  </si>
+  <si>
+    <t>Glossary</t>
+  </si>
+  <si>
+    <t>Glossary Path</t>
+  </si>
+  <si>
+    <t>MetaData</t>
+  </si>
+  <si>
+    <t>MetaData Path</t>
+  </si>
+  <si>
+    <t>Upload File</t>
+  </si>
+  <si>
+    <t>PDF/Doc Path</t>
+  </si>
+  <si>
+    <t>Upload Cover</t>
+  </si>
+  <si>
+    <t>Image Quality</t>
+  </si>
+  <si>
+    <t>Image Path</t>
+  </si>
+  <si>
+    <t>Upload TOC</t>
+  </si>
+  <si>
+    <t>TOC Path</t>
+  </si>
+  <si>
+    <t>Test Title</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Dynamic</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>96 dpi</t>
+  </si>
+  <si>
+    <t>Browse</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>High Quality</t>
   </si>
 </sst>
 </file>
@@ -124,9 +224,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -166,7 +266,66 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,29 +341,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,70 +371,18 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,6 +409,174 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -316,174 +584,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,17 +597,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,15 +621,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -547,26 +632,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -586,6 +651,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -594,153 +683,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -748,17 +848,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -872,8 +972,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C10:H20" totalsRowShown="0">
-  <autoFilter ref="C10:H20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C10:H22" totalsRowShown="0">
+  <autoFilter ref="C10:H22"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Environment" dataDxfId="0"/>
     <tableColumn id="2" name="Module" dataDxfId="1"/>
@@ -1144,64 +1244,64 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="37.8571428571429" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.2857142857143" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.2857142857143" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.5714285714286" style="3" customWidth="1"/>
-    <col min="5" max="5" width="66.7142857142857" style="3" customWidth="1"/>
-    <col min="6" max="6" width="37.5714285714286" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.4285714285714" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.5714285714286" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.14285714285714" style="3"/>
+    <col min="1" max="1" width="37.8571428571429" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.2857142857143" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.2857142857143" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.5714285714286" style="4" customWidth="1"/>
+    <col min="5" max="5" width="66.7142857142857" style="4" customWidth="1"/>
+    <col min="6" max="6" width="37.5714285714286" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.4285714285714" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.5714285714286" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.14285714285714" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:1">
+    <row r="3" s="4" customFormat="1" spans="1:1">
       <c r="A3" s="5"/>
     </row>
     <row r="10" spans="3:8">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1227,19 +1327,19 @@
     </row>
     <row r="12" spans="3:8">
       <c r="C12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="E12" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>13</v>
@@ -1247,19 +1347,19 @@
     </row>
     <row r="13" spans="3:8">
       <c r="C13" s="6" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>13</v>
@@ -1267,19 +1367,19 @@
     </row>
     <row r="14" spans="3:8">
       <c r="C14" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>13</v>
@@ -1287,41 +1387,41 @@
     </row>
     <row r="15" spans="3:8">
       <c r="C15" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="8" t="s">
+      <c r="G15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="3:8">
       <c r="C16" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1330,18 +1430,18 @@
         <v>22</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="F17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1350,59 +1450,99 @@
         <v>22</v>
       </c>
       <c r="D18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="C19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="C20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="D20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="3:8">
-      <c r="C19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="G20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="C21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="D21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8">
-      <c r="C20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="4" t="s">
+    </row>
+    <row r="22" spans="3:8">
+      <c r="C22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="E22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>29</v>
+      <c r="G22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1428,7 +1568,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A20"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1439,27 +1579,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
+      <c r="H1" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="24.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1428571428571" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.8571428571429" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.8571428571429" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7142857142857" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7142857142857" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5714285714286" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.4285714285714" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.57142857142857" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85714285714286" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7142857142857" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.8571428571429" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.14285714285714" style="1"/>
+    <col min="18" max="18" width="14" style="1" customWidth="1"/>
+    <col min="19" max="20" width="12.1428571428571" style="1" customWidth="1"/>
+    <col min="21" max="21" width="16" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="45" spans="1:23">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
+      <formula1>"Default,Image"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 L2 M2 O2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"English,Spanish,Hindi,Gujrati,Tamil,Castellano,Valenciano,Inglés,Catalán,Euskera,Gallego,Francés,Norwegian,Portugesse,Arabic,Marathi"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+      <formula1>"Other,Standard,Workbook,Auto Read Aloud"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2">
+      <formula1>"Browse,FileStack"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+      <formula1>"Dynamic,Lock Portrait,Lock Landscape"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+      <formula1>"96 dpi,125 dpi,150 dpi,300 dpi"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2">
+      <formula1>"High Quality,Low Quality"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DIS_2187(Sprint_34) and reader clients(AAO) are added.
</commit_message>
<xml_diff>
--- a/KitabooAutomation/testData/platformConfig.xlsx
+++ b/KitabooAutomation/testData/platformConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12510"/>
+    <workbookView windowWidth="28125" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="userConfig" sheetId="2" r:id="rId1"/>
@@ -224,9 +224,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -259,6 +259,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -272,8 +279,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,23 +295,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,14 +342,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,61 +393,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -409,13 +409,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,157 +547,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,11 +597,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,47 +627,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -684,6 +654,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -694,153 +679,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1246,8 +1246,8 @@
   <sheetPr/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1568,7 +1568,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1580,13 +1580,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>34</v>
@@ -1609,8 +1609,8 @@
   <sheetPr/>
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1739,7 +1739,6 @@
       <c r="Q2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
         <v>65</v>
       </c>
@@ -1749,11 +1748,8 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
-      <formula1>"Default,Image"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 L2 M2 O2">
-      <formula1>"Yes,No"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+      <formula1>"96 dpi,125 dpi,150 dpi,300 dpi"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
       <formula1>"English,Spanish,Hindi,Gujrati,Tamil,Castellano,Valenciano,Inglés,Catalán,Euskera,Gallego,Francés,Norwegian,Portugesse,Arabic,Marathi"</formula1>
@@ -1761,14 +1757,17 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
       <formula1>"Other,Standard,Workbook,Auto Read Aloud"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
+      <formula1>"Default,Image"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2">
       <formula1>"Browse,FileStack"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
       <formula1>"Dynamic,Lock Portrait,Lock Landscape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
-      <formula1>"96 dpi,125 dpi,150 dpi,300 dpi"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2 L2 M2 O2">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2">
       <formula1>"High Quality,Low Quality"</formula1>

</xml_diff>